<commit_message>
✨ SEO + Contenu réseaux sociaux : Automatisation administrative
- ✅ SEO : Ajout H1, hiérarchie headings, migration styles inline → CSS
- 📱 Contenu social media complet (LinkedIn, Facebook, Instagram)
- 🤖 17 prompts Sora/IA pour génération visuels
- 📚 Guides de publication et engagement

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Articles optimisés SEO/CALENDRIER_PUBLICATION_FLUXA.xlsx
+++ b/Articles optimisés SEO/CALENDRIER_PUBLICATION_FLUXA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Applications personnalisées\fluxa-artisans-automations-main\Articles optimisés SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98A494C-7E6D-4D3D-A166-F04361556C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DE92C-0F0C-418E-8730-F750AB56E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,7 +940,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1009,6 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -1892,7 +1893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30">
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="5" t="s">
         <v>61</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30">
+    <row r="18" spans="1:12" ht="30">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30">
+    <row r="20" spans="1:12" ht="30">
       <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
@@ -2032,7 +2033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30">
+    <row r="21" spans="1:12" ht="30">
       <c r="A21" s="5" t="s">
         <v>65</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30">
+    <row r="22" spans="1:12" ht="30">
       <c r="A22" s="6" t="s">
         <v>66</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30">
+    <row r="23" spans="1:12" ht="30">
       <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30">
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="3" t="s">
         <v>65</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30">
+    <row r="25" spans="1:12" ht="30">
       <c r="A25" s="4" t="s">
         <v>69</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30">
+    <row r="26" spans="1:12" ht="30">
       <c r="A26" s="2" t="s">
         <v>70</v>
       </c>
@@ -2242,7 +2243,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30">
+    <row r="27" spans="1:12" ht="30">
       <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30">
+    <row r="28" spans="1:12" ht="30">
       <c r="A28" s="4" t="s">
         <v>73</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30">
+    <row r="29" spans="1:12" ht="30">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30">
+    <row r="30" spans="1:12" ht="30">
       <c r="A30" s="3" t="s">
         <v>74</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30">
+    <row r="31" spans="1:12" ht="30">
       <c r="A31" s="4" t="s">
         <v>77</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30">
+    <row r="32" spans="1:12" ht="30">
       <c r="A32" s="5" t="s">
         <v>78</v>
       </c>
@@ -2451,6 +2452,7 @@
       <c r="K32" s="21" t="s">
         <v>21</v>
       </c>
+      <c r="L32" s="24"/>
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" s="2" t="s">

</xml_diff>

<commit_message>
Mise à jour locale
</commit_message>
<xml_diff>
--- a/Articles optimisés SEO/CALENDRIER_PUBLICATION_FLUXA.xlsx
+++ b/Articles optimisés SEO/CALENDRIER_PUBLICATION_FLUXA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Applications personnalisées\fluxa-artisans-automations-main\Articles optimisés SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DE92C-0F0C-418E-8730-F750AB56E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA5BD05-FED8-409F-8991-E35F55715835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="250">
   <si>
     <t>Date</t>
   </si>
@@ -940,7 +940,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1010,6 +1010,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,9 +1329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1509,8 +1524,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="30">
-      <c r="A6" s="3" t="s">
-        <v>36</v>
+      <c r="A6" s="25">
+        <v>45967</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -1539,8 +1554,8 @@
       <c r="J6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="19" t="s">
-        <v>21</v>
+      <c r="K6" s="26" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30">
@@ -1574,8 +1589,8 @@
       <c r="J7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="20" t="s">
-        <v>21</v>
+      <c r="K7" s="27" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
@@ -1609,8 +1624,8 @@
       <c r="J8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="21" t="s">
-        <v>21</v>
+      <c r="K8" s="29" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30">
@@ -1644,8 +1659,8 @@
       <c r="J9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="22" t="s">
-        <v>21</v>
+      <c r="K9" s="28" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30">
@@ -1714,8 +1729,8 @@
       <c r="J11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="19" t="s">
-        <v>21</v>
+      <c r="K11" s="26" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30">
@@ -1749,8 +1764,8 @@
       <c r="J12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="20" t="s">
-        <v>21</v>
+      <c r="K12" s="27" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30">
@@ -1784,8 +1799,8 @@
       <c r="J13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="21" t="s">
-        <v>21</v>
+      <c r="K13" s="29" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30">

</xml_diff>